<commit_message>
Hotel Module updated 13th nov
</commit_message>
<xml_diff>
--- a/src/main/java/gjha123/seleniumframework/resources/PassengerDetails.xlsx
+++ b/src/main/java/gjha123/seleniumframework/resources/PassengerDetails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ATB7X_SeleniumFrameworkDesign16October\seleniumframework\src\main\java\gjha123\seleniumframework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1922AE95-2974-4BB2-8069-E835B9C4684C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD736BC9-252B-445C-82C1-0895117F0BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Passenger1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Jha</t>
   </si>
@@ -41,20 +41,26 @@
     <t>LastNames</t>
   </si>
   <si>
-    <t>Pooja</t>
-  </si>
-  <si>
-    <t>Mishra</t>
-  </si>
-  <si>
     <t>Drashit</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>Gangesh</t>
+  </si>
+  <si>
+    <t>ujha777@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +71,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF1A1A1A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,15 +116,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -391,7 +408,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -422,32 +441,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD46B4-C038-46EB-9729-137D1D4529EB}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1234567890</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{6610EDDE-BEFA-4118-AC57-EBA161FD9823}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -470,7 +508,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>

</xml_diff>